<commit_message>
Konnect Bill Payment Verification Checks added
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/BeneDeletion.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/BeneDeletion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-10192020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-16122020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Case</t>
   </si>
@@ -78,16 +78,70 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>bene_op_type_query</t>
+  </si>
+  <si>
+    <t>bene_op_value</t>
+  </si>
+  <si>
+    <t>SELECT BENE_OPERATION_TYPE FROM DC_TRANSACTION DT where DT.TRANSACTION_ID='{TRANSACTION_ID}'</t>
+  </si>
+  <si>
+    <t>REMOVE</t>
+  </si>
+  <si>
+    <t>to_account_query</t>
+  </si>
+  <si>
+    <t>account_title_query</t>
+  </si>
+  <si>
+    <t>bene_bank_query</t>
+  </si>
+  <si>
+    <t>bene_id_tran_query</t>
+  </si>
+  <si>
+    <t>bene_id_query</t>
+  </si>
+  <si>
+    <t>SELECT K.TO_ACCOUNT FROM DC_TRANSACTION K WHERE K.TRANSACTION_ID = '{TRANSACTION_ID}'</t>
+  </si>
+  <si>
+    <t>SELECT K.FT_TO_ACCOUNT_TITLE FROM DC_TRANSACTION K WHERE K.TRANSACTION_ID = '{TRANSACTION_ID}'</t>
+  </si>
+  <si>
+    <t>SELECT K.BENEFICIARY_BANK FROM DC_TRANSACTION K WHERE K.TRANSACTION_ID = '{TRANSACTION_ID}'</t>
+  </si>
+  <si>
+    <t>SELECT BENEFICIARY_ID FROM DC_TRANSACTION K WHERE K.TRANSACTION_ID = '{TRANSACTION_ID}'</t>
+  </si>
+  <si>
+    <t>SELECT FUND_TRANSFER_BENEFICIARY_ID FROM DC_FUND_TRANSFER_BENEFICIARY K WHERE K.CUSTOMER_INFO_ID = (Select CUSTOMER_INFO_ID from DC_CUSTOMER_INFO L WHERE L.CUSTOMER_NAME = '{customer_name}' ) and K.ACCOUNT_NO = '{account_number}'</t>
+  </si>
+  <si>
+    <t>db_val</t>
+  </si>
+  <si>
+    <t>DIGITAL_CHANNEL_SEC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,9 +167,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,9 +467,17 @@
     <col min="6" max="6" width="78.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="72.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="204.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="100.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="100.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="244" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +502,32 @@
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -465,8 +552,32 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -490,6 +601,30 @@
       </c>
       <c r="H3" t="s">
         <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>